<commit_message>
add api CreateRoom & handle realtime FindOneAndGetLatestMessage by roomId
</commit_message>
<xml_diff>
--- a/Documents/ChatRealtime_Database.xlsx
+++ b/Documents/ChatRealtime_Database.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\S2_ICT_PROJECTS\Lab.SignalR\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\S2_ICT_PROJECTS\Lab.SignalR\Lab.SignalR_Chat.BE\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BD8AF2-F070-49C0-B1EA-A403E82D6B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357C1769-894F-4EB8-9986-481B679FB717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Users" sheetId="2" r:id="rId1"/>
     <sheet name="Messages" sheetId="51" r:id="rId2"/>
     <sheet name="Boxs" sheetId="52" r:id="rId3"/>
-    <sheet name="Groups" sheetId="53" r:id="rId4"/>
-    <sheet name="UserGroups" sheetId="54" r:id="rId5"/>
-    <sheet name="MessageGroups" sheetId="55" r:id="rId6"/>
+    <sheet name="Rooms" sheetId="53" r:id="rId4"/>
+    <sheet name="MessageRooms" sheetId="55" r:id="rId5"/>
+    <sheet name="UserGroups" sheetId="54" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="53">
   <si>
     <t>#</t>
   </si>
@@ -189,12 +189,6 @@
     <t>GroupId</t>
   </si>
   <si>
-    <t>UserGroupId</t>
-  </si>
-  <si>
-    <t>Id UserGroup</t>
-  </si>
-  <si>
     <t>Id User</t>
   </si>
   <si>
@@ -202,6 +196,9 @@
   </si>
   <si>
     <t>ObjectId</t>
+  </si>
+  <si>
+    <t>RoomId</t>
   </si>
 </sst>
 </file>
@@ -359,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -405,6 +402,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -414,9 +414,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,7 +786,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>7</v>
@@ -880,7 +878,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="19" t="s">
         <v>17</v>
       </c>
       <c r="G7" s="4"/>
@@ -1014,12 +1012,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -1061,7 +1059,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>7</v>
@@ -1344,12 +1342,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -1391,7 +1389,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>7</v>
@@ -1661,10 +1659,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,12 +1676,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
@@ -1725,7 +1723,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>7</v>
@@ -1808,17 +1806,643 @@
         <v>40</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="8" t="s">
         <v>45</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3E5795-1E00-4B3C-9C6C-A092966037A6}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:M23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+    </row>
+    <row r="2" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+    </row>
+    <row r="3" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39CCBB6-4B71-4488-833B-9A22AF6F7C93}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:M24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+    </row>
+    <row r="2" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+    </row>
+    <row r="3" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -1909,7 +2533,7 @@
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
@@ -1956,616 +2580,20 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E39CCBB6-4B71-4488-833B-9A22AF6F7C93}">
-  <sheetPr>
-    <tabColor theme="7" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:M24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-    </row>
-    <row r="2" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-    </row>
-    <row r="3" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3E5795-1E00-4B3C-9C6C-A092966037A6}">
-  <sheetPr>
-    <tabColor theme="7" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:M24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-    </row>
-    <row r="2" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-    </row>
-    <row r="3" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100418FFFDA85F47F4492A006938AD8A7A0" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="64ad0c7d6a41dc99318d6f9d64b6972c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="60e614c7-a9a6-4435-9132-2f84b3f93a8d" xmlns:ns3="147f8fa8-c619-4545-b8c0-d1c959b6e9f9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bafad0b654a91d11aa852bd6448dcf3e" ns2:_="" ns3:_="">
     <xsd:import namespace="60e614c7-a9a6-4435-9132-2f84b3f93a8d"/>
@@ -2794,15 +2822,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2815,6 +2834,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D41A3D-674D-46EC-AB67-3A7F25C0AD8E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C20E3A8-3B7D-4659-AD9B-046ECFD9D2D8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2833,14 +2860,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31D41A3D-674D-46EC-AB67-3A7F25C0AD8E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F1EC08E-4A7C-40B0-BECE-7A6BF435AD95}">
   <ds:schemaRefs>

</xml_diff>